<commit_message>
Finished getting the 7 parameter model figures and aic data
</commit_message>
<xml_diff>
--- a/AIC7parameters_FinalConfirmation_moredata.xlsx
+++ b/AIC7parameters_FinalConfirmation_moredata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Documents\MATLAB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E378848-7F76-4064-9854-0FD7B5E22CC4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC4C97DD-1B6E-4EC2-856F-97BDC907477C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11835" xr2:uid="{0C02BB13-C19D-4CA4-A317-53A2917ED159}"/>
   </bookViews>
@@ -387,244 +387,244 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1">
-        <v>2204.2292173355991</v>
+        <v>2200.2292173303581</v>
       </c>
       <c r="B1">
-        <v>1417.3586874575051</v>
+        <v>1413.0883371171401</v>
       </c>
       <c r="C1">
-        <v>1437.1682447638914</v>
+        <v>1433.2414832486022</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>2227.119236892242</v>
+        <v>2223.1192368732227</v>
       </c>
       <c r="B2">
-        <v>1482.0444984470635</v>
+        <v>1464.6353980171634</v>
       </c>
       <c r="C2">
-        <v>1329.642170635766</v>
+        <v>1430.9469458087237</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>2343.9137069531034</v>
+        <v>2339.9137069531034</v>
       </c>
       <c r="B3">
-        <v>1585.8915019097694</v>
+        <v>1581.8914897206105</v>
       </c>
       <c r="C3">
-        <v>1454.1273042076245</v>
+        <v>1450.1273560749194</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>2320.9625060647604</v>
+        <v>2316.96250606476</v>
       </c>
       <c r="B4">
-        <v>1774.3572927768962</v>
+        <v>1770.3572927336343</v>
       </c>
       <c r="C4">
-        <v>1703.6232104373485</v>
+        <v>1699.6232104240059</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>2422.6539934030502</v>
+        <v>2418.6539934030511</v>
       </c>
       <c r="B5">
-        <v>1668.5656738373048</v>
+        <v>1664.5656950833943</v>
       </c>
       <c r="C5">
-        <v>1625.8655676475478</v>
+        <v>1621.8655132393455</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>2360.7084402705214</v>
+        <v>2356.7084402705214</v>
       </c>
       <c r="B6">
-        <v>1774.6284616285989</v>
+        <v>1770.6284616285568</v>
       </c>
       <c r="C6">
-        <v>1784.4372524671107</v>
+        <v>1780.4372524670989</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>1992.9848474206722</v>
+        <v>1988.9848474206719</v>
       </c>
       <c r="B7">
-        <v>1567.0572054497206</v>
+        <v>1563.0572054573668</v>
       </c>
       <c r="C7">
-        <v>1484.3316331276569</v>
+        <v>1480.331633107181</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>2135.6712526944621</v>
+        <v>2131.6712526944602</v>
       </c>
       <c r="B8">
-        <v>1653.3121301485892</v>
+        <v>1649.3121108864455</v>
       </c>
       <c r="C8">
-        <v>1632.0931299514318</v>
+        <v>1628.0931546045269</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>2471.0153725374817</v>
+        <v>2467.015372537443</v>
       </c>
       <c r="B9">
-        <v>1788.308975545893</v>
+        <v>1784.3089756160193</v>
       </c>
       <c r="C9">
-        <v>1513.8937670922028</v>
+        <v>1509.8937671913866</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>2111.5944045181427</v>
+        <v>2107.594404518145</v>
       </c>
       <c r="B10">
-        <v>1370.7865883851514</v>
+        <v>1366.7866019700048</v>
       </c>
       <c r="C10">
-        <v>1287.1298050064961</v>
+        <v>1283.1297772827584</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>1970.0038839175647</v>
+        <v>1966.0038839175647</v>
       </c>
       <c r="B11">
-        <v>1416.2680734946873</v>
+        <v>1412.2680734948408</v>
       </c>
       <c r="C11">
-        <v>1298.5083154432789</v>
+        <v>1294.508315442717</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>2787.9537336891003</v>
+        <v>2783.9537336872691</v>
       </c>
       <c r="B12">
-        <v>2270.4374107467202</v>
+        <v>2266.437411002204</v>
       </c>
       <c r="C12">
-        <v>2036.7945281391187</v>
+        <v>2032.7945288481224</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>2315.1853411231882</v>
+        <v>2311.1853410557019</v>
       </c>
       <c r="B13">
-        <v>1739.7696417887169</v>
+        <v>1738.1827811731157</v>
       </c>
       <c r="C13">
-        <v>1820.7784890196647</v>
+        <v>1814.3571781233311</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>2593.0481324808579</v>
+        <v>2589.0481324808579</v>
       </c>
       <c r="B14">
-        <v>1922.3549806006286</v>
+        <v>1918.3549811213027</v>
       </c>
       <c r="C14">
-        <v>1702.6671162039202</v>
+        <v>1698.6671106768149</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>2508.3188623771198</v>
+        <v>2504.3188623771234</v>
       </c>
       <c r="B15">
-        <v>2047.727138686291</v>
+        <v>2043.7271445454799</v>
       </c>
       <c r="C15">
-        <v>1845.8802858112645</v>
+        <v>1841.8802398524401</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>2205.5211166450968</v>
+        <v>2201.5211166450968</v>
       </c>
       <c r="B16">
-        <v>1510.14576365271</v>
+        <v>1506.1457634936228</v>
       </c>
       <c r="C16">
-        <v>1270.5667535796013</v>
+        <v>1266.566756430175</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>2225.5448154950977</v>
+        <v>2221.5448154951432</v>
       </c>
       <c r="B17">
-        <v>1689.6426066041136</v>
+        <v>1685.6426137539731</v>
       </c>
       <c r="C17">
-        <v>1563.9267636753584</v>
+        <v>1559.9267688263026</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>2487.9072682735759</v>
+        <v>2483.9072682735809</v>
       </c>
       <c r="B18">
-        <v>2061.2767141880795</v>
+        <v>2057.2767182058769</v>
       </c>
       <c r="C18">
-        <v>1917.4119270443894</v>
+        <v>1913.4119084784868</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>1741.5582146654078</v>
+        <v>1737.5582140970034</v>
       </c>
       <c r="B19">
-        <v>1925.0538877583683</v>
+        <v>1921.0538878036466</v>
       </c>
       <c r="C19">
-        <v>1888.8258166955272</v>
+        <v>1884.8258167361525</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>2351.276345455467</v>
+        <v>2347.276345455467</v>
       </c>
       <c r="B20">
-        <v>1825.6044963322563</v>
+        <v>1821.6045095213988</v>
       </c>
       <c r="C20">
-        <v>1768.6831031667878</v>
+        <v>1764.6830779821748</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>2583.1100705929853</v>
+        <v>2579.110070587506</v>
       </c>
       <c r="B21">
-        <v>1907.065085287049</v>
+        <v>1903.0651052615717</v>
       </c>
       <c r="C21">
-        <v>1813.888239730006</v>
+        <v>1809.8882081724635</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>2448.3691933540563</v>
+        <v>2444.3691932947804</v>
       </c>
       <c r="B22">
-        <v>1890.2358444263193</v>
+        <v>1886.2358905041021</v>
       </c>
       <c r="C22">
-        <v>1645.6545097029136</v>
+        <v>1641.6541911979325</v>
       </c>
     </row>
   </sheetData>

</xml_diff>